<commit_message>
Fixing version and data initialization
</commit_message>
<xml_diff>
--- a/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
+++ b/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\base\common\base-common-std\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363C9BF9-039A-46E5-8014-095973E3E565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C97A18-37F6-44F3-BF1A-B99535E05547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A0A7498-F155-4A5F-9B3D-5648A71B0879}"/>
   </bookViews>
@@ -595,7 +595,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:XFD20"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,7 +1513,7 @@
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update of IOTC_LL_EQUATIONS for YFT
</commit_message>
<xml_diff>
--- a/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
+++ b/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\base\common\base-common-std\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfao-my.sharepoint.com/personal/emmanuel_chassot_fao_org/Documents/IOTC/TOOLS/R/IOTC_LIBS/R libs/base-common-std/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C97A18-37F6-44F3-BF1A-B99535E05547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{D3C97A18-37F6-44F3-BF1A-B99535E05547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2F2F5AD-C70F-4418-BFA5-8FFA7045A303}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A0A7498-F155-4A5F-9B3D-5648A71B0879}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A0A7498-F155-4A5F-9B3D-5648A71B0879}"/>
   </bookViews>
   <sheets>
     <sheet name="L_L" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="L_W" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">L_L!$A$1:$H$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">L_L!$A$1:$H$27</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="63">
   <si>
     <t>SPECIES</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>From the Access DB. Differs from the standard equation</t>
+  </si>
+  <si>
+    <t>IOTC 2005</t>
   </si>
 </sst>
 </file>
@@ -295,9 +298,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -335,7 +338,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -441,7 +444,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -583,7 +586,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -591,17 +594,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}">
-  <dimension ref="A1:H26"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -653,7 +658,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -676,7 +681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -699,7 +704,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -722,7 +727,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -745,7 +750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -768,7 +773,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -791,7 +796,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -814,7 +819,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -837,7 +842,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -860,7 +865,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -883,7 +888,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -909,7 +914,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -935,7 +940,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -961,7 +966,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -987,7 +992,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1013,7 +1018,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1039,7 +1044,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1065,7 +1070,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1091,7 +1096,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1114,7 +1119,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1140,7 +1145,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1166,7 +1171,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -1193,17 +1198,91 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="1"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="1"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1.2129000000000001</v>
+      </c>
+      <c r="F25" s="3">
+        <v>18.190999999999999</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1.2211000000000001</v>
+      </c>
+      <c r="F26" s="3">
+        <v>10.733000000000001</v>
+      </c>
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1.3693</v>
+      </c>
+      <c r="F27" s="3">
+        <v>21.399000000000001</v>
+      </c>
+      <c r="G27" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H24" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}"/>
+  <autoFilter ref="A1:H27" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="BET"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1215,7 +1294,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Addition of 2 length-length questions for YFT and 1 for BET
</commit_message>
<xml_diff>
--- a/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
+++ b/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfao-my.sharepoint.com/personal/emmanuel_chassot_fao_org/Documents/IOTC/TOOLS/R/IOTC_LIBS/R libs/base-common-std/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{D3C97A18-37F6-44F3-BF1A-B99535E05547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2F2F5AD-C70F-4418-BFA5-8FFA7045A303}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{D3C97A18-37F6-44F3-BF1A-B99535E05547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE7350EB-4BE3-43C9-BA4F-1C36FBCAE797}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A0A7498-F155-4A5F-9B3D-5648A71B0879}"/>
   </bookViews>
@@ -295,6 +295,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -599,7 +603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD26"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +639,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -658,7 +662,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1197,7 +1201,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1223,7 +1227,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1249,7 +1253,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1279,7 +1283,7 @@
   <autoFilter ref="A1:H27" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}">
     <filterColumn colId="0">
       <filters>
-        <filter val="BET"/>
+        <filter val="YFT"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Addition of 2 length-length parameters for ALB
</commit_message>
<xml_diff>
--- a/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
+++ b/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfao-my.sharepoint.com/personal/emmanuel_chassot_fao_org/Documents/IOTC/TOOLS/R/IOTC_LIBS/R libs/base-common-std/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\r-libs\base-common-std\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{D3C97A18-37F6-44F3-BF1A-B99535E05547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE7350EB-4BE3-43C9-BA4F-1C36FBCAE797}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C808A2B1-2F39-485F-954C-B5A755160764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A0A7498-F155-4A5F-9B3D-5648A71B0879}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A0A7498-F155-4A5F-9B3D-5648A71B0879}"/>
   </bookViews>
   <sheets>
     <sheet name="L_L" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="64">
   <si>
     <t>SPECIES</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>IOTC 2005</t>
+  </si>
+  <si>
+    <t>Dhurmeea2016</t>
   </si>
 </sst>
 </file>
@@ -295,10 +298,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,12 +597,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <selection pane="bottomLeft" activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +637,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -685,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -708,7 +706,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -731,7 +729,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -754,7 +752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -777,7 +775,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -800,7 +798,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -823,7 +821,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -846,7 +844,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -869,7 +867,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -892,7 +890,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -918,7 +916,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -944,7 +942,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -970,7 +968,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -996,7 +994,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1022,7 +1020,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1048,7 +1046,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1074,7 +1072,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1100,7 +1098,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1123,7 +1121,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1149,7 +1147,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1175,7 +1173,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -1201,7 +1199,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1279,14 +1277,60 @@
         <v>62</v>
       </c>
     </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0.26779999999999998</v>
+      </c>
+      <c r="F28">
+        <v>5.4938000000000002</v>
+      </c>
+      <c r="G28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0.7016</v>
+      </c>
+      <c r="F29">
+        <v>0.61739999999999995</v>
+      </c>
+      <c r="G29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H27" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="YFT"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H27" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Major update in morphometric parameters
</commit_message>
<xml_diff>
--- a/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
+++ b/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\r-libs\base-common-std\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data-processing\iotc-lib-base-common-std\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C808A2B1-2F39-485F-954C-B5A755160764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D51BFD-9658-43B2-B277-6560C4AB28D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A0A7498-F155-4A5F-9B3D-5648A71B0879}"/>
   </bookViews>
@@ -18,9 +18,9 @@
     <sheet name="L_W" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">L_L!$A$1:$H$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">L_L!$A$1:$H$95</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,9 +28,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="75">
   <si>
     <t>SPECIES</t>
   </si>
@@ -61,12 +64,18 @@
     <t>BET</t>
   </si>
   <si>
+    <t>FLC</t>
+  </si>
+  <si>
     <t>FL</t>
   </si>
   <si>
     <t>IDENTITY</t>
   </si>
   <si>
+    <t>FLCT</t>
+  </si>
+  <si>
     <t>FLUT</t>
   </si>
   <si>
@@ -94,9 +103,15 @@
     <t>GGT</t>
   </si>
   <si>
+    <t>FLB</t>
+  </si>
+  <si>
     <t>LDF</t>
   </si>
   <si>
+    <t>LDFT</t>
+  </si>
+  <si>
     <t>SQUARED</t>
   </si>
   <si>
@@ -139,12 +154,24 @@
     <t>PAL</t>
   </si>
   <si>
+    <t>PALT</t>
+  </si>
+  <si>
     <t>PCL</t>
   </si>
   <si>
+    <t>PCLT</t>
+  </si>
+  <si>
     <t>HDD</t>
   </si>
   <si>
+    <t>CKUT</t>
+  </si>
+  <si>
+    <t>EFUT</t>
+  </si>
+  <si>
     <t>EQ_ID</t>
   </si>
   <si>
@@ -230,6 +257,15 @@
   </si>
   <si>
     <t>Dhurmeea2016</t>
+  </si>
+  <si>
+    <t>Oliveira2005</t>
+  </si>
+  <si>
+    <t>MLD</t>
+  </si>
+  <si>
+    <t>Champagnat1974 - corrected from LDF to MLD</t>
   </si>
 </sst>
 </file>
@@ -257,12 +293,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -277,12 +319,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,18 +640,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}">
-  <dimension ref="A1:H29"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N25" sqref="N25"/>
+      <selection pane="bottomLeft" activeCell="M96" sqref="M96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -631,10 +680,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -642,695 +691,2228 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>21.451080000000001</v>
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
       </c>
       <c r="F2" s="3">
-        <v>5.28756</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="3">
-        <v>2.0758999999999999</v>
+        <v>0</v>
       </c>
       <c r="F3" s="3">
-        <v>1.1513</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>0.8972</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>-4.6673</v>
+        <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="3">
-        <v>0.90390000000000004</v>
+        <v>0</v>
       </c>
       <c r="F5" s="3">
-        <v>-7.2480000000000002</v>
+        <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="3">
-        <v>0</v>
+      <c r="E6" s="2">
+        <v>21.451080000000001</v>
       </c>
       <c r="F6" s="3">
-        <v>0</v>
+        <v>5.28756</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2.0758999999999999</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1.1513</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2.0758999999999999</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.1513</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.8972</v>
+      </c>
+      <c r="F18" s="3">
+        <v>-4.6673</v>
+      </c>
+      <c r="G18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.8972</v>
+      </c>
+      <c r="F19" s="3">
+        <v>-4.6673</v>
+      </c>
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.8972</v>
+      </c>
+      <c r="F20" s="3">
+        <v>-4.6673</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.90390000000000004</v>
+      </c>
+      <c r="F22" s="3">
+        <v>-7.2480000000000002</v>
+      </c>
+      <c r="G22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.90390000000000004</v>
+      </c>
+      <c r="F23" s="3">
+        <v>-7.2480000000000002</v>
+      </c>
+      <c r="G23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.90390000000000004</v>
+      </c>
+      <c r="F24" s="3">
+        <v>-7.2480000000000002</v>
+      </c>
+      <c r="G24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
         <v>0.88449999999999995</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F28" s="3">
         <v>-3.7025000000000001</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.88449999999999995</v>
+      </c>
+      <c r="F29" s="3">
+        <v>-3.7025000000000001</v>
+      </c>
+      <c r="G29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.88449999999999995</v>
+      </c>
+      <c r="F30" s="3">
+        <v>-3.7025000000000001</v>
+      </c>
+      <c r="G30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
         <v>0.80869999999999997</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F35" s="3">
         <v>8.6712000000000007</v>
       </c>
-      <c r="G8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="G35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1.55108</v>
+      </c>
+      <c r="F36" s="3">
+        <v>13.5025</v>
+      </c>
+      <c r="G36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1.55108</v>
+      </c>
+      <c r="F37" s="3">
+        <v>13.5025</v>
+      </c>
+      <c r="G37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="F38" s="3">
+        <v>10.449</v>
+      </c>
+      <c r="G38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="F39" s="3">
+        <v>10.449</v>
+      </c>
+      <c r="G39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3">
+        <v>2.5407000000000002</v>
+      </c>
+      <c r="F40" s="3">
+        <v>25.698</v>
+      </c>
+      <c r="G40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3">
+        <v>2.5407000000000002</v>
+      </c>
+      <c r="F41" s="3">
+        <v>25.698</v>
+      </c>
+      <c r="G41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1.2398</v>
+      </c>
+      <c r="F42" s="3">
+        <v>11.204000000000001</v>
+      </c>
+      <c r="G42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1.2398</v>
+      </c>
+      <c r="F43" s="3">
+        <v>11.204000000000001</v>
+      </c>
+      <c r="G43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.55108</v>
-      </c>
-      <c r="F9" s="3">
-        <v>13.5025</v>
-      </c>
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.0660000000000001</v>
-      </c>
-      <c r="F10" s="3">
-        <v>10.449</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0</v>
+      </c>
+      <c r="G48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0</v>
+      </c>
+      <c r="G50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0</v>
+      </c>
+      <c r="G51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0</v>
+      </c>
+      <c r="G53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" s="3">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0</v>
+      </c>
+      <c r="G54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0</v>
+      </c>
+      <c r="G55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0</v>
+      </c>
+      <c r="G56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3">
+        <v>0</v>
+      </c>
+      <c r="G57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3">
+        <v>0</v>
+      </c>
+      <c r="G58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0</v>
+      </c>
+      <c r="E59" s="3">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3">
+        <v>0</v>
+      </c>
+      <c r="G59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0</v>
+      </c>
+      <c r="E60" s="3">
+        <v>0</v>
+      </c>
+      <c r="F60" s="3">
+        <v>0</v>
+      </c>
+      <c r="G60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0</v>
+      </c>
+      <c r="E61" s="3">
+        <v>0</v>
+      </c>
+      <c r="F61" s="3">
+        <v>0</v>
+      </c>
+      <c r="G61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0</v>
+      </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0</v>
+      </c>
+      <c r="G62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>45</v>
+      </c>
+      <c r="B63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0</v>
+      </c>
+      <c r="E63" s="3">
+        <v>0</v>
+      </c>
+      <c r="F63" s="3">
+        <v>0</v>
+      </c>
+      <c r="G63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>49</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0</v>
+      </c>
+      <c r="E64" s="3">
+        <v>0</v>
+      </c>
+      <c r="F64" s="3">
+        <v>0</v>
+      </c>
+      <c r="G64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+      <c r="E65" s="3">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3">
+        <v>0</v>
+      </c>
+      <c r="G65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>49</v>
+      </c>
+      <c r="B66" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0</v>
+      </c>
+      <c r="E66" s="3">
+        <v>0</v>
+      </c>
+      <c r="F66" s="3">
+        <v>0</v>
+      </c>
+      <c r="G66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>49</v>
+      </c>
+      <c r="B67" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+      <c r="E67" s="3">
+        <v>0</v>
+      </c>
+      <c r="F67" s="3">
+        <v>0</v>
+      </c>
+      <c r="G67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>59</v>
+      </c>
+      <c r="B68" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0</v>
+      </c>
+      <c r="E68" s="3">
+        <v>0</v>
+      </c>
+      <c r="F68" s="3">
+        <v>0</v>
+      </c>
+      <c r="G68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0</v>
+      </c>
+      <c r="E69" s="3">
+        <v>0</v>
+      </c>
+      <c r="F69" s="3">
+        <v>0</v>
+      </c>
+      <c r="G69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>50</v>
+      </c>
+      <c r="B70" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0</v>
+      </c>
+      <c r="E70" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="F70" s="3">
+        <v>-0.8</v>
+      </c>
+      <c r="G70" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3">
-        <v>2.5407000000000002</v>
-      </c>
-      <c r="F11" s="3">
-        <v>25.698</v>
-      </c>
-      <c r="G11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1.2398</v>
-      </c>
-      <c r="F12" s="3">
-        <v>11.204000000000001</v>
-      </c>
-      <c r="G12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.98</v>
-      </c>
-      <c r="F13" s="3">
-        <v>-0.8</v>
-      </c>
-      <c r="G13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="H70" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>50</v>
+      </c>
+      <c r="B71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="1">
+        <v>1</v>
+      </c>
+      <c r="E71" s="3">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="F71" s="3">
+        <v>0.39560000000000001</v>
+      </c>
+      <c r="G71" t="s">
+        <v>55</v>
+      </c>
+      <c r="H71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1</v>
+      </c>
+      <c r="E72" s="3">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="F72" s="3">
+        <v>0.39560000000000001</v>
+      </c>
+      <c r="G72" t="s">
+        <v>55</v>
+      </c>
+      <c r="H72" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" t="s">
+        <v>51</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1">
+        <v>1</v>
+      </c>
+      <c r="E73" s="3">
+        <v>0.85609999999999997</v>
+      </c>
+      <c r="F73" s="3">
+        <v>-4.5541999999999998</v>
+      </c>
+      <c r="G73" t="s">
+        <v>32</v>
+      </c>
+      <c r="H73" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.90749999999999997</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.39560000000000001</v>
-      </c>
-      <c r="G14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="B74" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0</v>
+      </c>
+      <c r="E74" s="3">
+        <v>0</v>
+      </c>
+      <c r="F74" s="3">
+        <v>0</v>
+      </c>
+      <c r="G74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>56</v>
+      </c>
+      <c r="B75" t="s">
+        <v>20</v>
+      </c>
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0</v>
+      </c>
+      <c r="E75" s="3">
+        <v>0</v>
+      </c>
+      <c r="F75" s="3">
+        <v>0</v>
+      </c>
+      <c r="G75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>56</v>
+      </c>
+      <c r="B76" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0</v>
+      </c>
+      <c r="E76" s="3">
+        <v>0</v>
+      </c>
+      <c r="F76" s="3">
+        <v>0</v>
+      </c>
+      <c r="G76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>56</v>
+      </c>
+      <c r="B77" t="s">
+        <v>51</v>
+      </c>
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="1">
+        <v>1</v>
+      </c>
+      <c r="E77" s="3">
+        <v>0.81130000000000002</v>
+      </c>
+      <c r="F77" s="3">
+        <v>1.0883</v>
+      </c>
+      <c r="G77" t="s">
+        <v>32</v>
+      </c>
+      <c r="H77" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>53</v>
+      </c>
+      <c r="B78" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0</v>
+      </c>
+      <c r="E78" s="3">
+        <v>0</v>
+      </c>
+      <c r="F78" s="3">
+        <v>0</v>
+      </c>
+      <c r="G78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>53</v>
+      </c>
+      <c r="B79" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" s="1">
+        <v>1</v>
+      </c>
+      <c r="E79" s="3">
+        <v>0.86019999999999996</v>
+      </c>
+      <c r="F79" s="3">
+        <v>7.2885</v>
+      </c>
+      <c r="G79" t="s">
+        <v>32</v>
+      </c>
+      <c r="H79" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>54</v>
+      </c>
+      <c r="B80" t="s">
+        <v>38</v>
+      </c>
+      <c r="C80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1</v>
+      </c>
+      <c r="E80" s="3">
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="F80" s="3">
+        <v>1.99</v>
+      </c>
+      <c r="G80" t="s">
+        <v>32</v>
+      </c>
+      <c r="H80" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.85609999999999997</v>
-      </c>
-      <c r="F15" s="3">
-        <v>-4.5541999999999998</v>
-      </c>
-      <c r="G15" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.81130000000000002</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1.0883</v>
-      </c>
-      <c r="G16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0.86019999999999996</v>
-      </c>
-      <c r="F17" s="3">
-        <v>7.2885</v>
-      </c>
-      <c r="G17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1.0980000000000001</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="G18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="B81" t="s">
+        <v>51</v>
+      </c>
+      <c r="C81" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1</v>
+      </c>
+      <c r="E81" s="3">
         <v>0.80830000000000002</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F81" s="3">
         <v>7.1478000000000002</v>
       </c>
-      <c r="G19" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="G81" t="s">
+        <v>32</v>
+      </c>
+      <c r="H81" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="1">
+        <v>0</v>
+      </c>
+      <c r="E82" s="3">
+        <v>0</v>
+      </c>
+      <c r="F82" s="3">
+        <v>0</v>
+      </c>
+      <c r="G82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>52</v>
+      </c>
+      <c r="B83" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1</v>
+      </c>
+      <c r="E83" s="3">
         <v>0.96799999999999997</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F83" s="3">
         <v>-0.97299999999999998</v>
       </c>
-      <c r="G20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="G83" t="s">
+        <v>32</v>
+      </c>
+      <c r="H83" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" t="s">
+        <v>38</v>
+      </c>
+      <c r="C84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="1">
+        <v>1</v>
+      </c>
+      <c r="E84" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F84" s="3">
         <v>0.76600000000000001</v>
       </c>
-      <c r="G21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3">
+      <c r="G84" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>52</v>
+      </c>
+      <c r="B85" t="s">
+        <v>39</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="1">
+        <v>1</v>
+      </c>
+      <c r="E85" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="G85" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>52</v>
+      </c>
+      <c r="B86" t="s">
+        <v>51</v>
+      </c>
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="1">
+        <v>1</v>
+      </c>
+      <c r="E86" s="3">
         <v>0.90469999999999995</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F86" s="3">
         <v>0.59630000000000005</v>
       </c>
-      <c r="G22" t="s">
-        <v>28</v>
-      </c>
-      <c r="H22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="G86" t="s">
+        <v>32</v>
+      </c>
+      <c r="H86" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>62</v>
+      </c>
+      <c r="B87" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0</v>
+      </c>
+      <c r="E87" s="3">
+        <v>0</v>
+      </c>
+      <c r="F87" s="3">
+        <v>0</v>
+      </c>
+      <c r="G87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>62</v>
+      </c>
+      <c r="B88" t="s">
+        <v>51</v>
+      </c>
+      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="1">
+        <v>1</v>
+      </c>
+      <c r="E88" s="3">
         <v>0.7994</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F88" s="3">
         <v>-1.0546</v>
       </c>
-      <c r="G23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" s="3">
+      <c r="G88" t="s">
+        <v>32</v>
+      </c>
+      <c r="H88" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>63</v>
+      </c>
+      <c r="B89" t="s">
+        <v>51</v>
+      </c>
+      <c r="C89" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="1">
+        <v>1</v>
+      </c>
+      <c r="E89" s="3">
         <v>0.80389999999999995</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F89" s="3">
         <v>-4.3490000000000002</v>
       </c>
-      <c r="G24" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="G89" t="s">
+        <v>32</v>
+      </c>
+      <c r="H89" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>18</v>
+      </c>
+      <c r="B90" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" s="1">
+        <v>1</v>
+      </c>
+      <c r="E90" s="3">
+        <v>1.2211000000000001</v>
+      </c>
+      <c r="F90" s="3">
+        <v>10.733000000000001</v>
+      </c>
+      <c r="G90" t="s">
+        <v>32</v>
+      </c>
+      <c r="H90" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91" t="s">
+        <v>35</v>
+      </c>
+      <c r="C91" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" s="1">
+        <v>1</v>
+      </c>
+      <c r="E91" s="3">
+        <v>1.3693</v>
+      </c>
+      <c r="F91" s="3">
+        <v>21.399000000000001</v>
+      </c>
+      <c r="G91" t="s">
+        <v>32</v>
+      </c>
+      <c r="H91" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="1">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>0.26779999999999998</v>
+      </c>
+      <c r="F92">
+        <v>5.4938000000000002</v>
+      </c>
+      <c r="G92" t="s">
+        <v>34</v>
+      </c>
+      <c r="H92" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>24</v>
+      </c>
+      <c r="B93" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" s="1">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>0.7016</v>
+      </c>
+      <c r="F93">
+        <v>0.61739999999999995</v>
+      </c>
+      <c r="G93" t="s">
+        <v>34</v>
+      </c>
+      <c r="H93" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>6</v>
       </c>
-      <c r="B25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3">
+      <c r="B94" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" t="s">
+        <v>51</v>
+      </c>
+      <c r="D94" s="1">
+        <v>1</v>
+      </c>
+      <c r="E94" s="3">
+        <v>1.0455000000000001</v>
+      </c>
+      <c r="F94" s="3">
+        <v>6.5838999999999999</v>
+      </c>
+      <c r="G94" t="s">
+        <v>32</v>
+      </c>
+      <c r="H94" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" t="s">
+        <v>38</v>
+      </c>
+      <c r="C95" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="1">
+        <v>1</v>
+      </c>
+      <c r="E95" s="3">
         <v>1.2129000000000001</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F95" s="3">
         <v>18.190999999999999</v>
       </c>
-      <c r="G25" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1.2211000000000001</v>
-      </c>
-      <c r="F26" s="3">
-        <v>10.733000000000001</v>
-      </c>
-      <c r="G26" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1.3693</v>
-      </c>
-      <c r="F27" s="3">
-        <v>21.399000000000001</v>
-      </c>
-      <c r="G27" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>0.26779999999999998</v>
-      </c>
-      <c r="F28">
-        <v>5.4938000000000002</v>
-      </c>
-      <c r="G28" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>0.7016</v>
-      </c>
-      <c r="F29">
-        <v>0.61739999999999995</v>
-      </c>
-      <c r="G29" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" t="s">
-        <v>63</v>
+      <c r="G95" t="s">
+        <v>32</v>
+      </c>
+      <c r="H95" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H27" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}"/>
+  <autoFilter ref="A1:H95" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="BET"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1342,7 +2924,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,10 +2953,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1382,10 +2964,10 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1397,18 +2979,18 @@
         <v>0.30085909999999999</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -1420,18 +3002,18 @@
         <v>0.30123490000000003</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1443,18 +3025,18 @@
         <v>3.0792999999999999</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1466,18 +3048,18 @@
         <v>0.30944199999999999</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1489,18 +3071,18 @@
         <v>0.28337699999999999</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -1512,18 +3094,18 @@
         <v>0.30041699999999999</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1535,18 +3117,18 @@
         <v>0.30041699999999999</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1558,18 +3140,18 @@
         <v>0.34716599999999997</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1581,18 +3163,18 @@
         <v>3.1880000000000002</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -1604,18 +3186,18 @@
         <v>3.1880000000000002</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -1627,7 +3209,7 @@
         <v>3.137</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1661,7 +3243,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1673,10 +3255,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1684,13 +3266,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1702,7 +3284,7 @@
         <v>3.0121099999999998</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1710,13 +3292,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1">
         <v>1.1299999999999999</v>
@@ -1728,21 +3310,21 @@
         <v>3.0415414023</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1754,21 +3336,21 @@
         <v>2.9666999999999999</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
       <c r="E5" s="1">
         <v>1.1299999999999999</v>
@@ -1780,21 +3362,21 @@
         <v>3.126843987</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -1806,21 +3388,21 @@
         <v>3.3929200000000002</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -1832,21 +3414,21 @@
         <v>3.3929200000000002</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -1858,21 +3440,21 @@
         <v>2.7513999999999998</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -1884,21 +3466,21 @@
         <v>2.7513999999999998</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1910,21 +3492,21 @@
         <v>3.2134</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -1936,21 +3518,21 @@
         <v>3.2134</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -1962,21 +3544,21 @@
         <v>2.9885100000000002</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1988,21 +3570,21 @@
         <v>2.9885100000000002</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -2014,21 +3596,21 @@
         <v>3.3096700000000001</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -2040,21 +3622,21 @@
         <v>3.3096700000000001</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -2066,21 +3648,21 @@
         <v>3.41344</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -2092,21 +3674,21 @@
         <v>3.41344</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -2118,21 +3700,21 @@
         <v>2.5242900000000001</v>
       </c>
       <c r="H18" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -2144,21 +3726,21 @@
         <v>2.5242900000000001</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -2170,21 +3752,21 @@
         <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -2196,21 +3778,21 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -2222,21 +3804,21 @@
         <v>3</v>
       </c>
       <c r="H22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -2248,21 +3830,21 @@
         <v>3</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
@@ -2274,21 +3856,21 @@
         <v>2.9</v>
       </c>
       <c r="H24" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -2300,21 +3882,21 @@
         <v>2.9</v>
       </c>
       <c r="H25" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -2326,21 +3908,21 @@
         <v>2.83</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
@@ -2352,21 +3934,21 @@
         <v>2.83</v>
       </c>
       <c r="H27" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
@@ -2378,21 +3960,21 @@
         <v>2.9001999999999999</v>
       </c>
       <c r="H28" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -2404,21 +3986,21 @@
         <v>2.9001999999999999</v>
       </c>
       <c r="H29" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -2430,21 +4012,21 @@
         <v>2.8940000000000001</v>
       </c>
       <c r="H30" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -2456,21 +4038,21 @@
         <v>2.8940000000000001</v>
       </c>
       <c r="H31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
@@ -2482,21 +4064,21 @@
         <v>3.1313</v>
       </c>
       <c r="H32" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -2508,21 +4090,21 @@
         <v>3.1313</v>
       </c>
       <c r="H33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -2534,21 +4116,21 @@
         <v>3.1406999999999998</v>
       </c>
       <c r="H34" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
@@ -2560,21 +4142,21 @@
         <v>3.1406999999999998</v>
       </c>
       <c r="H35" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -2586,21 +4168,21 @@
         <v>2.9245000000000001</v>
       </c>
       <c r="H36" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -2612,21 +4194,21 @@
         <v>2.9245000000000001</v>
       </c>
       <c r="H37" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -2638,21 +4220,21 @@
         <v>2.9641000000000002</v>
       </c>
       <c r="H38" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -2664,21 +4246,21 @@
         <v>2.9641000000000002</v>
       </c>
       <c r="H39" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -2690,21 +4272,21 @@
         <v>2.9220999999999999</v>
       </c>
       <c r="H40" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -2716,21 +4298,21 @@
         <v>2.9220999999999999</v>
       </c>
       <c r="H41" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -2742,21 +4324,21 @@
         <v>3.0802</v>
       </c>
       <c r="H42" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
@@ -2768,21 +4350,21 @@
         <v>3.0802</v>
       </c>
       <c r="H43" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
@@ -2794,24 +4376,24 @@
         <v>2.5188000000000001</v>
       </c>
       <c r="H44" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I44" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D45" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
@@ -2823,24 +4405,24 @@
         <v>2.5188000000000001</v>
       </c>
       <c r="H45" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I45" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
@@ -2852,24 +4434,24 @@
         <v>2.5188000000000001</v>
       </c>
       <c r="H46" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I46" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D47" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E47" s="1">
         <v>1</v>
@@ -2881,24 +4463,24 @@
         <v>2.5188000000000001</v>
       </c>
       <c r="H47" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I47" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E48" s="1">
         <v>1</v>
@@ -2910,24 +4492,24 @@
         <v>3.1406999999999998</v>
       </c>
       <c r="H48" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I48" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E49" s="1">
         <v>1</v>
@@ -2939,24 +4521,24 @@
         <v>3.1406999999999998</v>
       </c>
       <c r="H49" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I49" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E50" s="1">
         <v>1</v>
@@ -2968,24 +4550,24 @@
         <v>2.1156000000000001</v>
       </c>
       <c r="H50" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I50" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E51" s="1">
         <v>1</v>
@@ -2997,24 +4579,24 @@
         <v>2.1156000000000001</v>
       </c>
       <c r="H51" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I51" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E52" s="1">
         <v>1</v>
@@ -3026,24 +4608,24 @@
         <v>3.1406999999999998</v>
       </c>
       <c r="H52" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I52" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E53" s="1">
         <v>1</v>
@@ -3055,24 +4637,24 @@
         <v>3.1406999999999998</v>
       </c>
       <c r="H53" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I53" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D54" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E54" s="1">
         <v>1</v>
@@ -3084,24 +4666,24 @@
         <v>3.0669</v>
       </c>
       <c r="H54" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -3113,24 +4695,24 @@
         <v>3.0669</v>
       </c>
       <c r="H55" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I55" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D56" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E56" s="1">
         <v>1</v>
@@ -3142,24 +4724,24 @@
         <v>3.0669</v>
       </c>
       <c r="H56" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I56" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D57" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E57" s="1">
         <v>1</v>
@@ -3171,10 +4753,10 @@
         <v>3.0669</v>
       </c>
       <c r="H57" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I57" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inversion of FL-TL equation for BET for consistency
</commit_message>
<xml_diff>
--- a/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
+++ b/data-raw/IOTC_DETERMINISTIC_EQUATIONS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data-processing\iotc-lib-base-common-std\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D51BFD-9658-43B2-B277-6560C4AB28D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE707EE-E208-460A-B669-12C060A75AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A0A7498-F155-4A5F-9B3D-5648A71B0879}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A0A7498-F155-4A5F-9B3D-5648A71B0879}"/>
   </bookViews>
   <sheets>
     <sheet name="L_L" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="L_W" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">L_L!$A$1:$H$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">L_L!$A$1:$H$94</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -640,12 +640,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M96" sqref="M96"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A94" sqref="A94:XFD94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +803,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -827,7 +826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -850,7 +849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -873,7 +872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -896,7 +895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -919,7 +918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -942,7 +941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -965,7 +964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -988,7 +987,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1034,7 +1033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1057,7 +1056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1080,7 +1079,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1103,7 +1102,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1126,7 +1125,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1149,7 +1148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1172,7 +1171,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1195,7 +1194,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1218,7 +1217,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1241,7 +1240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1264,7 +1263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1310,7 +1309,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1333,7 +1332,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1356,7 +1355,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1379,7 +1378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -1402,7 +1401,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1425,7 +1424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1448,7 +1447,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -1471,7 +1470,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1494,7 +1493,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -1540,7 +1539,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -1563,7 +1562,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1586,7 +1585,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1609,7 +1608,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -1632,7 +1631,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -1655,7 +1654,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1678,7 +1677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1701,7 +1700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1724,7 +1723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -1747,7 +1746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1770,7 +1769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -1793,7 +1792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -1816,7 +1815,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -1839,7 +1838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -1862,7 +1861,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -1885,7 +1884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -1908,7 +1907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -1931,7 +1930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -1954,7 +1953,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -2000,7 +1999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -2023,7 +2022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>45</v>
       </c>
@@ -2046,7 +2045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>45</v>
       </c>
@@ -2069,7 +2068,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>45</v>
       </c>
@@ -2092,7 +2091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>45</v>
       </c>
@@ -2115,7 +2114,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>49</v>
       </c>
@@ -2138,7 +2137,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>49</v>
       </c>
@@ -2161,7 +2160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>49</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -2207,7 +2206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -2230,7 +2229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>50</v>
       </c>
@@ -2253,7 +2252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>50</v>
       </c>
@@ -2279,7 +2278,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>50</v>
       </c>
@@ -2305,7 +2304,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>50</v>
       </c>
@@ -2331,7 +2330,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>50</v>
       </c>
@@ -2357,7 +2356,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>57</v>
       </c>
@@ -2380,7 +2379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>56</v>
       </c>
@@ -2403,7 +2402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>56</v>
       </c>
@@ -2426,7 +2425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>56</v>
       </c>
@@ -2452,7 +2451,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>53</v>
       </c>
@@ -2475,7 +2474,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>53</v>
       </c>
@@ -2501,7 +2500,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>54</v>
       </c>
@@ -2527,7 +2526,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>61</v>
       </c>
@@ -2553,7 +2552,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>52</v>
       </c>
@@ -2576,7 +2575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>52</v>
       </c>
@@ -2602,7 +2601,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>52</v>
       </c>
@@ -2625,7 +2624,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>52</v>
       </c>
@@ -2648,7 +2647,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>52</v>
       </c>
@@ -2674,7 +2673,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>62</v>
       </c>
@@ -2697,7 +2696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>62</v>
       </c>
@@ -2723,7 +2722,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>63</v>
       </c>
@@ -2749,7 +2748,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>18</v>
       </c>
@@ -2775,7 +2774,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>18</v>
       </c>
@@ -2801,7 +2800,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>24</v>
       </c>
@@ -2827,7 +2826,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>24</v>
       </c>
@@ -2858,25 +2857,25 @@
         <v>6</v>
       </c>
       <c r="B94" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C94" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="D94" s="1">
         <v>1</v>
       </c>
       <c r="E94" s="3">
-        <v>1.0455000000000001</v>
+        <v>1.2129000000000001</v>
       </c>
       <c r="F94" s="3">
-        <v>6.5838999999999999</v>
+        <v>18.190999999999999</v>
       </c>
       <c r="G94" t="s">
         <v>32</v>
       </c>
       <c r="H94" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -2884,7 +2883,7 @@
         <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
@@ -2892,27 +2891,21 @@
       <c r="D95" s="1">
         <v>1</v>
       </c>
-      <c r="E95" s="3">
-        <v>1.2129000000000001</v>
-      </c>
-      <c r="F95" s="3">
-        <v>18.190999999999999</v>
+      <c r="E95">
+        <v>0.95648015303682443</v>
+      </c>
+      <c r="F95">
+        <v>-6.2973696795791483</v>
       </c>
       <c r="G95" t="s">
         <v>32</v>
       </c>
       <c r="H95" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H95" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="BET"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H94" xr:uid="{B94DDCA6-578B-4B20-B64C-EF257705AB91}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>